<commit_message>
added score for presentations of cse 101 section 8 & 9
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101 Non CSE/results_cse101_sec8.xlsx
+++ b/FALL 19/CSE 101 Non CSE/results_cse101_sec8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\CSE 101 Non CSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBAAAAD-9CA7-4437-8244-9702E469DB88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E775CC4-FDEA-4306-A6DD-02C5BA648DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="mid2" sheetId="3" r:id="rId3"/>
     <sheet name="mid_total" sheetId="4" r:id="rId4"/>
     <sheet name="final" sheetId="5" r:id="rId5"/>
+    <sheet name="presentation" sheetId="6" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -243,16 +247,29 @@
   <si>
     <t>Marks 6</t>
   </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -288,6 +305,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,7 +316,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -306,34 +324,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D52BF41C-157E-415A-A241-C642C3EFA20F}"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -497,6 +641,602 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>193011189</v>
+          </cell>
+          <cell r="C2">
+            <v>4</v>
+          </cell>
+          <cell r="D2">
+            <v>193011189</v>
+          </cell>
+          <cell r="E2">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>193011035</v>
+          </cell>
+          <cell r="C3">
+            <v>4</v>
+          </cell>
+          <cell r="D3">
+            <v>193011035</v>
+          </cell>
+          <cell r="E3">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>193011181</v>
+          </cell>
+          <cell r="C4">
+            <v>4</v>
+          </cell>
+          <cell r="D4">
+            <v>193011181</v>
+          </cell>
+          <cell r="E4">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>193011166</v>
+          </cell>
+          <cell r="C5">
+            <v>3.5</v>
+          </cell>
+          <cell r="D5">
+            <v>193011166</v>
+          </cell>
+          <cell r="E5">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>191012011</v>
+          </cell>
+          <cell r="D6">
+            <v>191012011</v>
+          </cell>
+          <cell r="E6">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>193013015</v>
+          </cell>
+          <cell r="D7">
+            <v>193013015</v>
+          </cell>
+          <cell r="E7">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>192011003</v>
+          </cell>
+          <cell r="D8">
+            <v>192011003</v>
+          </cell>
+          <cell r="E8">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>193013021</v>
+          </cell>
+          <cell r="C10">
+            <v>5</v>
+          </cell>
+          <cell r="D10">
+            <v>193013021</v>
+          </cell>
+          <cell r="E10">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>183016004</v>
+          </cell>
+          <cell r="C11">
+            <v>5</v>
+          </cell>
+          <cell r="D11">
+            <v>183016004</v>
+          </cell>
+          <cell r="E11">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>193011116</v>
+          </cell>
+          <cell r="C12">
+            <v>3</v>
+          </cell>
+          <cell r="D12">
+            <v>193011116</v>
+          </cell>
+          <cell r="E12">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>193016004</v>
+          </cell>
+          <cell r="C13">
+            <v>3</v>
+          </cell>
+          <cell r="D13">
+            <v>193016004</v>
+          </cell>
+          <cell r="E13">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>192011116</v>
+          </cell>
+          <cell r="D14">
+            <v>192011116</v>
+          </cell>
+          <cell r="E14">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>193013043</v>
+          </cell>
+          <cell r="D15">
+            <v>193013043</v>
+          </cell>
+          <cell r="E15">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>193013055</v>
+          </cell>
+          <cell r="D16">
+            <v>193013055</v>
+          </cell>
+          <cell r="E16">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>193013038</v>
+          </cell>
+          <cell r="C17">
+            <v>3</v>
+          </cell>
+          <cell r="D17">
+            <v>193013038</v>
+          </cell>
+          <cell r="E17">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>193013006</v>
+          </cell>
+          <cell r="D19">
+            <v>193013006</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>173013015</v>
+          </cell>
+          <cell r="D20">
+            <v>173013015</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>193011117</v>
+          </cell>
+          <cell r="D21">
+            <v>193011117</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>193011194</v>
+          </cell>
+          <cell r="D22">
+            <v>193011194</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>193011176</v>
+          </cell>
+          <cell r="D23">
+            <v>193011176</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>193011185</v>
+          </cell>
+          <cell r="D24">
+            <v>193011185</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>193013005</v>
+          </cell>
+          <cell r="D25">
+            <v>193013005</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>193011025</v>
+          </cell>
+          <cell r="C27">
+            <v>4.5</v>
+          </cell>
+          <cell r="D27">
+            <v>193011025</v>
+          </cell>
+          <cell r="E27">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>193011152</v>
+          </cell>
+          <cell r="C28">
+            <v>2.5</v>
+          </cell>
+          <cell r="D28">
+            <v>193011152</v>
+          </cell>
+          <cell r="E28">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29">
+            <v>193011005</v>
+          </cell>
+          <cell r="C29">
+            <v>3</v>
+          </cell>
+          <cell r="D29">
+            <v>193011005</v>
+          </cell>
+          <cell r="E29">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30">
+            <v>193011075</v>
+          </cell>
+          <cell r="C30">
+            <v>4</v>
+          </cell>
+          <cell r="D30">
+            <v>193011075</v>
+          </cell>
+          <cell r="E30">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31">
+            <v>193011123</v>
+          </cell>
+          <cell r="C31">
+            <v>2.5</v>
+          </cell>
+          <cell r="D31">
+            <v>193011123</v>
+          </cell>
+          <cell r="E31">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32">
+            <v>193011122</v>
+          </cell>
+          <cell r="C32">
+            <v>2.5</v>
+          </cell>
+          <cell r="D32">
+            <v>193011122</v>
+          </cell>
+          <cell r="E32">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33">
+            <v>191011053</v>
+          </cell>
+          <cell r="D33">
+            <v>191011053</v>
+          </cell>
+          <cell r="E33">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35">
+            <v>191012060</v>
+          </cell>
+          <cell r="D35">
+            <v>191012060</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36">
+            <v>193011105</v>
+          </cell>
+          <cell r="D36">
+            <v>193011105</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37">
+            <v>193013050</v>
+          </cell>
+          <cell r="D37">
+            <v>193013050</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39">
+            <v>193013088</v>
+          </cell>
+          <cell r="C39">
+            <v>4</v>
+          </cell>
+          <cell r="D39">
+            <v>193013088</v>
+          </cell>
+          <cell r="E39">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40">
+            <v>193013008</v>
+          </cell>
+          <cell r="C40">
+            <v>4.5</v>
+          </cell>
+          <cell r="D40">
+            <v>193013008</v>
+          </cell>
+          <cell r="E40">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41">
+            <v>192011156</v>
+          </cell>
+          <cell r="C41">
+            <v>4</v>
+          </cell>
+          <cell r="D41">
+            <v>192011156</v>
+          </cell>
+          <cell r="E41">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42">
+            <v>193013046</v>
+          </cell>
+          <cell r="C42">
+            <v>3.5</v>
+          </cell>
+          <cell r="D42">
+            <v>193013046</v>
+          </cell>
+          <cell r="E42">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43">
+            <v>193013030</v>
+          </cell>
+          <cell r="C43">
+            <v>4</v>
+          </cell>
+          <cell r="D43">
+            <v>193013030</v>
+          </cell>
+          <cell r="E43">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44">
+            <v>193013096</v>
+          </cell>
+          <cell r="C44">
+            <v>4.5</v>
+          </cell>
+          <cell r="D44">
+            <v>193013096</v>
+          </cell>
+          <cell r="E44">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45">
+            <v>182013026</v>
+          </cell>
+          <cell r="D45">
+            <v>182013026</v>
+          </cell>
+          <cell r="E45">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46">
+            <v>193016002</v>
+          </cell>
+          <cell r="C46">
+            <v>3</v>
+          </cell>
+          <cell r="D46">
+            <v>193016002</v>
+          </cell>
+          <cell r="E46">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="B48">
+            <v>193011069</v>
+          </cell>
+          <cell r="C48">
+            <v>3.5</v>
+          </cell>
+          <cell r="D48">
+            <v>193011069</v>
+          </cell>
+          <cell r="E48">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="B49">
+            <v>193011133</v>
+          </cell>
+          <cell r="C49">
+            <v>2.5</v>
+          </cell>
+          <cell r="D49">
+            <v>193011133</v>
+          </cell>
+          <cell r="E49">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50">
+            <v>191011226</v>
+          </cell>
+          <cell r="C50">
+            <v>2.5</v>
+          </cell>
+          <cell r="D50">
+            <v>191011226</v>
+          </cell>
+          <cell r="E50">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="B51">
+            <v>182014039</v>
+          </cell>
+          <cell r="C51">
+            <v>3</v>
+          </cell>
+          <cell r="D51">
+            <v>182014039</v>
+          </cell>
+          <cell r="E51">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52">
+            <v>191011023</v>
+          </cell>
+          <cell r="C52">
+            <v>3</v>
+          </cell>
+          <cell r="D52">
+            <v>191011023</v>
+          </cell>
+          <cell r="E52">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53">
+            <v>193011128</v>
+          </cell>
+          <cell r="D53">
+            <v>193011128</v>
+          </cell>
+          <cell r="E53">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54">
+            <v>191012061</v>
+          </cell>
+          <cell r="D54">
+            <v>191012061</v>
+          </cell>
+          <cell r="E54">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="B55">
+            <v>192011051</v>
+          </cell>
+          <cell r="C55">
+            <v>2.5</v>
+          </cell>
+          <cell r="D55">
+            <v>192011051</v>
+          </cell>
+          <cell r="E55">
+            <v>6</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8759,7 +9499,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8768,8 +9508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355CD6C3-0968-416E-AD99-DA1E04F24285}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11520,7 +12260,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C2:C49">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
@@ -11543,4 +12283,1408 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36981321-2A1A-46DA-A7F6-4FDFF056C86A}">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="10" customWidth="1"/>
+    <col min="3" max="7" width="14.77734375" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>191011023</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="26">
+        <f>VLOOKUP(A2,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D2" s="26">
+        <f>VLOOKUP(A2,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E2" s="27">
+        <f>C2+D2</f>
+        <v>9</v>
+      </c>
+      <c r="F2" s="24">
+        <f>(E2/E$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="G2" s="18" t="str">
+        <f>IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>191011053</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="26">
+        <f>VLOOKUP(A3,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="26">
+        <f>VLOOKUP(A3,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E3" s="27">
+        <f>C3+D3</f>
+        <v>8.5</v>
+      </c>
+      <c r="F3" s="24">
+        <f>(E3/E$50)*100</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="G3" s="18" t="str">
+        <f>IF(F3&gt;94,"A+",IF(F3&gt;84,"A",IF(F3&gt;79,"A-",IF(F3&gt;74,"B+",IF(F3&gt;69,"B",IF(F3&gt;64,"B-",IF(F3&gt;59,"C+",IF(F3&gt;54,"C",IF(F3&gt;49,"D","F")))))))))</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>191011226</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="26">
+        <f>VLOOKUP(A4,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="26">
+        <f>VLOOKUP(A4,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E4" s="27">
+        <f>C4+D4</f>
+        <v>8.5</v>
+      </c>
+      <c r="F4" s="24">
+        <f>(E4/E$50)*100</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="G4" s="18" t="str">
+        <f>IF(F4&gt;94,"A+",IF(F4&gt;84,"A",IF(F4&gt;79,"A-",IF(F4&gt;74,"B+",IF(F4&gt;69,"B",IF(F4&gt;64,"B-",IF(F4&gt;59,"C+",IF(F4&gt;54,"C",IF(F4&gt;49,"D","F")))))))))</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>192011003</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="26">
+        <f>VLOOKUP(A5,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="26">
+        <f>VLOOKUP(A5,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="27">
+        <f>C5+D5</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="24">
+        <f>(E5/E$50)*100</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="G5" s="18" t="str">
+        <f>IF(F5&gt;94,"A+",IF(F5&gt;84,"A",IF(F5&gt;79,"A-",IF(F5&gt;74,"B+",IF(F5&gt;69,"B",IF(F5&gt;64,"B-",IF(F5&gt;59,"C+",IF(F5&gt;54,"C",IF(F5&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>192011051</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="26">
+        <f>VLOOKUP(A6,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="26">
+        <f>VLOOKUP(A6,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="27">
+        <f>C6+D6</f>
+        <v>8.5</v>
+      </c>
+      <c r="F6" s="24">
+        <f>(E6/E$50)*100</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="G6" s="18" t="str">
+        <f>IF(F6&gt;94,"A+",IF(F6&gt;84,"A",IF(F6&gt;79,"A-",IF(F6&gt;74,"B+",IF(F6&gt;69,"B",IF(F6&gt;64,"B-",IF(F6&gt;59,"C+",IF(F6&gt;54,"C",IF(F6&gt;49,"D","F")))))))))</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>192011116</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="26">
+        <f>VLOOKUP(A7,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="26">
+        <f>VLOOKUP(A7,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E7" s="27">
+        <f>C7+D7</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="24">
+        <f>(E7/E$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="G7" s="18" t="str">
+        <f>IF(F7&gt;94,"A+",IF(F7&gt;84,"A",IF(F7&gt;79,"A-",IF(F7&gt;74,"B+",IF(F7&gt;69,"B",IF(F7&gt;64,"B-",IF(F7&gt;59,"C+",IF(F7&gt;54,"C",IF(F7&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>192011156</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="26">
+        <f>VLOOKUP(A8,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="26">
+        <f>VLOOKUP(A8,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E8" s="27">
+        <f>C8+D8</f>
+        <v>12</v>
+      </c>
+      <c r="F8" s="24">
+        <f>(E8/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G8" s="18" t="str">
+        <f>IF(F8&gt;94,"A+",IF(F8&gt;84,"A",IF(F8&gt;79,"A-",IF(F8&gt;74,"B+",IF(F8&gt;69,"B",IF(F8&gt;64,"B-",IF(F8&gt;59,"C+",IF(F8&gt;54,"C",IF(F8&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>193011005</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="26">
+        <f>VLOOKUP(A9,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="26">
+        <f>VLOOKUP(A9,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E9" s="27">
+        <f>C9+D9</f>
+        <v>11.5</v>
+      </c>
+      <c r="F9" s="24">
+        <f>(E9/E$50)*100</f>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="G9" s="18" t="str">
+        <f>IF(F9&gt;94,"A+",IF(F9&gt;84,"A",IF(F9&gt;79,"A-",IF(F9&gt;74,"B+",IF(F9&gt;69,"B",IF(F9&gt;64,"B-",IF(F9&gt;59,"C+",IF(F9&gt;54,"C",IF(F9&gt;49,"D","F")))))))))</f>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>193011025</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="26">
+        <f>VLOOKUP(A10,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="26">
+        <f>VLOOKUP(A10,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E10" s="27">
+        <f>C10+D10</f>
+        <v>13</v>
+      </c>
+      <c r="F10" s="24">
+        <f>(E10/E$50)*100</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="G10" s="18" t="str">
+        <f>IF(F10&gt;94,"A+",IF(F10&gt;84,"A",IF(F10&gt;79,"A-",IF(F10&gt;74,"B+",IF(F10&gt;69,"B",IF(F10&gt;64,"B-",IF(F10&gt;59,"C+",IF(F10&gt;54,"C",IF(F10&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>193011035</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="26">
+        <f>VLOOKUP(A11,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D11" s="26">
+        <f>VLOOKUP(A11,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="27">
+        <f>C11+D11</f>
+        <v>12</v>
+      </c>
+      <c r="F11" s="24">
+        <f>(E11/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G11" s="18" t="str">
+        <f>IF(F11&gt;94,"A+",IF(F11&gt;84,"A",IF(F11&gt;79,"A-",IF(F11&gt;74,"B+",IF(F11&gt;69,"B",IF(F11&gt;64,"B-",IF(F11&gt;59,"C+",IF(F11&gt;54,"C",IF(F11&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="19">
+        <v>193011069</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="26">
+        <f>VLOOKUP(A12,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="26">
+        <f>VLOOKUP(A12,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E12" s="27">
+        <f>C12+D12</f>
+        <v>9.5</v>
+      </c>
+      <c r="F12" s="24">
+        <f>(E12/E$50)*100</f>
+        <v>63.333333333333329</v>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>IF(F12&gt;94,"A+",IF(F12&gt;84,"A",IF(F12&gt;79,"A-",IF(F12&gt;74,"B+",IF(F12&gt;69,"B",IF(F12&gt;64,"B-",IF(F12&gt;59,"C+",IF(F12&gt;54,"C",IF(F12&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>193011075</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="26">
+        <f>VLOOKUP(A13,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D13" s="26">
+        <f>VLOOKUP(A13,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E13" s="27">
+        <f>C13+D13</f>
+        <v>12.5</v>
+      </c>
+      <c r="F13" s="24">
+        <f>(E13/E$50)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="G13" s="18" t="str">
+        <f>IF(F13&gt;94,"A+",IF(F13&gt;84,"A",IF(F13&gt;79,"A-",IF(F13&gt;74,"B+",IF(F13&gt;69,"B",IF(F13&gt;64,"B-",IF(F13&gt;59,"C+",IF(F13&gt;54,"C",IF(F13&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>193011105</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="26">
+        <f>VLOOKUP(A14,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="26">
+        <f>VLOOKUP(A14,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="27">
+        <f>C14+D14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="24">
+        <f>(E14/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="18" t="str">
+        <f>IF(F14&gt;94,"A+",IF(F14&gt;84,"A",IF(F14&gt;79,"A-",IF(F14&gt;74,"B+",IF(F14&gt;69,"B",IF(F14&gt;64,"B-",IF(F14&gt;59,"C+",IF(F14&gt;54,"C",IF(F14&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>193011116</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="26">
+        <f>VLOOKUP(A15,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="26">
+        <f>VLOOKUP(A15,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E15" s="27">
+        <f>C15+D15</f>
+        <v>12</v>
+      </c>
+      <c r="F15" s="24">
+        <f>(E15/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G15" s="18" t="str">
+        <f>IF(F15&gt;94,"A+",IF(F15&gt;84,"A",IF(F15&gt;79,"A-",IF(F15&gt;74,"B+",IF(F15&gt;69,"B",IF(F15&gt;64,"B-",IF(F15&gt;59,"C+",IF(F15&gt;54,"C",IF(F15&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>193011117</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="26">
+        <f>VLOOKUP(A16,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="26">
+        <f>VLOOKUP(A16,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="27">
+        <f>C16+D16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="24">
+        <f>(E16/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="18" t="str">
+        <f>IF(F16&gt;94,"A+",IF(F16&gt;84,"A",IF(F16&gt;79,"A-",IF(F16&gt;74,"B+",IF(F16&gt;69,"B",IF(F16&gt;64,"B-",IF(F16&gt;59,"C+",IF(F16&gt;54,"C",IF(F16&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>193011122</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="26">
+        <f>VLOOKUP(A17,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="26">
+        <f>VLOOKUP(A17,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E17" s="27">
+        <f>C17+D17</f>
+        <v>11</v>
+      </c>
+      <c r="F17" s="24">
+        <f>(E17/E$50)*100</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="G17" s="18" t="str">
+        <f>IF(F17&gt;94,"A+",IF(F17&gt;84,"A",IF(F17&gt;79,"A-",IF(F17&gt;74,"B+",IF(F17&gt;69,"B",IF(F17&gt;64,"B-",IF(F17&gt;59,"C+",IF(F17&gt;54,"C",IF(F17&gt;49,"D","F")))))))))</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>193011123</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="26">
+        <f>VLOOKUP(A18,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="26">
+        <f>VLOOKUP(A18,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E18" s="27">
+        <f>C18+D18</f>
+        <v>11</v>
+      </c>
+      <c r="F18" s="24">
+        <f>(E18/E$50)*100</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="G18" s="18" t="str">
+        <f>IF(F18&gt;94,"A+",IF(F18&gt;84,"A",IF(F18&gt;79,"A-",IF(F18&gt;74,"B+",IF(F18&gt;69,"B",IF(F18&gt;64,"B-",IF(F18&gt;59,"C+",IF(F18&gt;54,"C",IF(F18&gt;49,"D","F")))))))))</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>193011128</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="26">
+        <f>VLOOKUP(A19,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="26">
+        <f>VLOOKUP(A19,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E19" s="27">
+        <f>C19+D19</f>
+        <v>6</v>
+      </c>
+      <c r="F19" s="24">
+        <f>(E19/E$50)*100</f>
+        <v>40</v>
+      </c>
+      <c r="G19" s="18" t="str">
+        <f>IF(F19&gt;94,"A+",IF(F19&gt;84,"A",IF(F19&gt;79,"A-",IF(F19&gt;74,"B+",IF(F19&gt;69,"B",IF(F19&gt;64,"B-",IF(F19&gt;59,"C+",IF(F19&gt;54,"C",IF(F19&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>193011133</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="26">
+        <f>VLOOKUP(A20,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D20" s="26">
+        <f>VLOOKUP(A20,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E20" s="27">
+        <f>C20+D20</f>
+        <v>8.5</v>
+      </c>
+      <c r="F20" s="24">
+        <f>(E20/E$50)*100</f>
+        <v>56.666666666666664</v>
+      </c>
+      <c r="G20" s="18" t="str">
+        <f>IF(F20&gt;94,"A+",IF(F20&gt;84,"A",IF(F20&gt;79,"A-",IF(F20&gt;74,"B+",IF(F20&gt;69,"B",IF(F20&gt;64,"B-",IF(F20&gt;59,"C+",IF(F20&gt;54,"C",IF(F20&gt;49,"D","F")))))))))</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>193011152</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="26">
+        <f>VLOOKUP(A21,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D21" s="26">
+        <f>VLOOKUP(A21,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="E21" s="27">
+        <f>C21+D21</f>
+        <v>11</v>
+      </c>
+      <c r="F21" s="24">
+        <f>(E21/E$50)*100</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="G21" s="18" t="str">
+        <f>IF(F21&gt;94,"A+",IF(F21&gt;84,"A",IF(F21&gt;79,"A-",IF(F21&gt;74,"B+",IF(F21&gt;69,"B",IF(F21&gt;64,"B-",IF(F21&gt;59,"C+",IF(F21&gt;54,"C",IF(F21&gt;49,"D","F")))))))))</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="19">
+        <v>193011166</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="26">
+        <f>VLOOKUP(A22,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D22" s="26">
+        <f>VLOOKUP(A22,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E22" s="27">
+        <f>C22+D22</f>
+        <v>11.5</v>
+      </c>
+      <c r="F22" s="24">
+        <f>(E22/E$50)*100</f>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="G22" s="18" t="str">
+        <f>IF(F22&gt;94,"A+",IF(F22&gt;84,"A",IF(F22&gt;79,"A-",IF(F22&gt;74,"B+",IF(F22&gt;69,"B",IF(F22&gt;64,"B-",IF(F22&gt;59,"C+",IF(F22&gt;54,"C",IF(F22&gt;49,"D","F")))))))))</f>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>193011176</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="26">
+        <f>VLOOKUP(A23,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="26">
+        <f>VLOOKUP(A23,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="27">
+        <f>C23+D23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <f>(E23/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="18" t="str">
+        <f>IF(F23&gt;94,"A+",IF(F23&gt;84,"A",IF(F23&gt;79,"A-",IF(F23&gt;74,"B+",IF(F23&gt;69,"B",IF(F23&gt;64,"B-",IF(F23&gt;59,"C+",IF(F23&gt;54,"C",IF(F23&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="19">
+        <v>193011181</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="26">
+        <f>VLOOKUP(A24,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="26">
+        <f>VLOOKUP(A24,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E24" s="27">
+        <f>C24+D24</f>
+        <v>12</v>
+      </c>
+      <c r="F24" s="24">
+        <f>(E24/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G24" s="18" t="str">
+        <f>IF(F24&gt;94,"A+",IF(F24&gt;84,"A",IF(F24&gt;79,"A-",IF(F24&gt;74,"B+",IF(F24&gt;69,"B",IF(F24&gt;64,"B-",IF(F24&gt;59,"C+",IF(F24&gt;54,"C",IF(F24&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="19">
+        <v>193011185</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="26">
+        <f>VLOOKUP(A25,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="26">
+        <f>VLOOKUP(A25,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="27">
+        <f>C25+D25</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <f>(E25/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="18" t="str">
+        <f>IF(F25&gt;94,"A+",IF(F25&gt;84,"A",IF(F25&gt;79,"A-",IF(F25&gt;74,"B+",IF(F25&gt;69,"B",IF(F25&gt;64,"B-",IF(F25&gt;59,"C+",IF(F25&gt;54,"C",IF(F25&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="19">
+        <v>193011189</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="26">
+        <f>VLOOKUP(A26,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D26" s="26">
+        <f>VLOOKUP(A26,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E26" s="27">
+        <f>C26+D26</f>
+        <v>12</v>
+      </c>
+      <c r="F26" s="24">
+        <f>(E26/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G26" s="18" t="str">
+        <f>IF(F26&gt;94,"A+",IF(F26&gt;84,"A",IF(F26&gt;79,"A-",IF(F26&gt;74,"B+",IF(F26&gt;69,"B",IF(F26&gt;64,"B-",IF(F26&gt;59,"C+",IF(F26&gt;54,"C",IF(F26&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="19">
+        <v>193011194</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="26">
+        <f>VLOOKUP(A27,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="26">
+        <f>VLOOKUP(A27,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="27">
+        <f>C27+D27</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="24">
+        <f>(E27/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="18" t="str">
+        <f>IF(F27&gt;94,"A+",IF(F27&gt;84,"A",IF(F27&gt;79,"A-",IF(F27&gt;74,"B+",IF(F27&gt;69,"B",IF(F27&gt;64,"B-",IF(F27&gt;59,"C+",IF(F27&gt;54,"C",IF(F27&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="19">
+        <v>191012011</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="26">
+        <f>VLOOKUP(A28,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="26">
+        <f>VLOOKUP(A28,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E28" s="27">
+        <f>C28+D28</f>
+        <v>8</v>
+      </c>
+      <c r="F28" s="24">
+        <f>(E28/E$50)*100</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="G28" s="18" t="str">
+        <f>IF(F28&gt;94,"A+",IF(F28&gt;84,"A",IF(F28&gt;79,"A-",IF(F28&gt;74,"B+",IF(F28&gt;69,"B",IF(F28&gt;64,"B-",IF(F28&gt;59,"C+",IF(F28&gt;54,"C",IF(F28&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
+        <v>191012060</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="26">
+        <f>VLOOKUP(A29,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="26">
+        <f>VLOOKUP(A29,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="27">
+        <f>C29+D29</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="24">
+        <f>(E29/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="18" t="str">
+        <f>IF(F29&gt;94,"A+",IF(F29&gt;84,"A",IF(F29&gt;79,"A-",IF(F29&gt;74,"B+",IF(F29&gt;69,"B",IF(F29&gt;64,"B-",IF(F29&gt;59,"C+",IF(F29&gt;54,"C",IF(F29&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>191012061</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="26">
+        <f>VLOOKUP(A30,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="26">
+        <f>VLOOKUP(A30,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E30" s="27">
+        <f>C30+D30</f>
+        <v>6</v>
+      </c>
+      <c r="F30" s="24">
+        <f>(E30/E$50)*100</f>
+        <v>40</v>
+      </c>
+      <c r="G30" s="18" t="str">
+        <f>IF(F30&gt;94,"A+",IF(F30&gt;84,"A",IF(F30&gt;79,"A-",IF(F30&gt;74,"B+",IF(F30&gt;69,"B",IF(F30&gt;64,"B-",IF(F30&gt;59,"C+",IF(F30&gt;54,"C",IF(F30&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="19">
+        <v>173013015</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="26">
+        <f>VLOOKUP(A31,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="26">
+        <f>VLOOKUP(A31,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="27">
+        <f>C31+D31</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <f>(E31/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="18" t="str">
+        <f>IF(F31&gt;94,"A+",IF(F31&gt;84,"A",IF(F31&gt;79,"A-",IF(F31&gt;74,"B+",IF(F31&gt;69,"B",IF(F31&gt;64,"B-",IF(F31&gt;59,"C+",IF(F31&gt;54,"C",IF(F31&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
+        <v>182013026</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="26">
+        <f>VLOOKUP(A32,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="26">
+        <f>VLOOKUP(A32,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E32" s="27">
+        <f>C32+D32</f>
+        <v>8</v>
+      </c>
+      <c r="F32" s="24">
+        <f>(E32/E$50)*100</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="G32" s="18" t="str">
+        <f>IF(F32&gt;94,"A+",IF(F32&gt;84,"A",IF(F32&gt;79,"A-",IF(F32&gt;74,"B+",IF(F32&gt;69,"B",IF(F32&gt;64,"B-",IF(F32&gt;59,"C+",IF(F32&gt;54,"C",IF(F32&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="19">
+        <v>193013005</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="26">
+        <f>VLOOKUP(A33,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="26">
+        <f>VLOOKUP(A33,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="27">
+        <f>C33+D33</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="24">
+        <f>(E33/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="18" t="str">
+        <f>IF(F33&gt;94,"A+",IF(F33&gt;84,"A",IF(F33&gt;79,"A-",IF(F33&gt;74,"B+",IF(F33&gt;69,"B",IF(F33&gt;64,"B-",IF(F33&gt;59,"C+",IF(F33&gt;54,"C",IF(F33&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>193013006</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="26">
+        <f>VLOOKUP(A34,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="26">
+        <f>VLOOKUP(A34,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="27">
+        <f>C34+D34</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <f>(E34/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="18" t="str">
+        <f>IF(F34&gt;94,"A+",IF(F34&gt;84,"A",IF(F34&gt;79,"A-",IF(F34&gt;74,"B+",IF(F34&gt;69,"B",IF(F34&gt;64,"B-",IF(F34&gt;59,"C+",IF(F34&gt;54,"C",IF(F34&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="19">
+        <v>193013008</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="26">
+        <f>VLOOKUP(A35,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D35" s="26">
+        <f>VLOOKUP(A35,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E35" s="27">
+        <f>C35+D35</f>
+        <v>12.5</v>
+      </c>
+      <c r="F35" s="24">
+        <f>(E35/E$50)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="G35" s="18" t="str">
+        <f>IF(F35&gt;94,"A+",IF(F35&gt;84,"A",IF(F35&gt;79,"A-",IF(F35&gt;74,"B+",IF(F35&gt;69,"B",IF(F35&gt;64,"B-",IF(F35&gt;59,"C+",IF(F35&gt;54,"C",IF(F35&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="19">
+        <v>193013015</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="26">
+        <f>VLOOKUP(A36,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="26">
+        <f>VLOOKUP(A36,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E36" s="27">
+        <f>C36+D36</f>
+        <v>8</v>
+      </c>
+      <c r="F36" s="24">
+        <f>(E36/E$50)*100</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="G36" s="18" t="str">
+        <f>IF(F36&gt;94,"A+",IF(F36&gt;84,"A",IF(F36&gt;79,"A-",IF(F36&gt;74,"B+",IF(F36&gt;69,"B",IF(F36&gt;64,"B-",IF(F36&gt;59,"C+",IF(F36&gt;54,"C",IF(F36&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="19">
+        <v>193013021</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="26">
+        <f>VLOOKUP(A37,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D37" s="26">
+        <f>VLOOKUP(A37,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E37" s="27">
+        <f>C37+D37</f>
+        <v>14</v>
+      </c>
+      <c r="F37" s="24">
+        <f>(E37/E$50)*100</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="G37" s="18" t="str">
+        <f>IF(F37&gt;94,"A+",IF(F37&gt;84,"A",IF(F37&gt;79,"A-",IF(F37&gt;74,"B+",IF(F37&gt;69,"B",IF(F37&gt;64,"B-",IF(F37&gt;59,"C+",IF(F37&gt;54,"C",IF(F37&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="19">
+        <v>193013030</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="26">
+        <f>VLOOKUP(A38,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D38" s="26">
+        <f>VLOOKUP(A38,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E38" s="27">
+        <f>C38+D38</f>
+        <v>12</v>
+      </c>
+      <c r="F38" s="24">
+        <f>(E38/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G38" s="18" t="str">
+        <f>IF(F38&gt;94,"A+",IF(F38&gt;84,"A",IF(F38&gt;79,"A-",IF(F38&gt;74,"B+",IF(F38&gt;69,"B",IF(F38&gt;64,"B-",IF(F38&gt;59,"C+",IF(F38&gt;54,"C",IF(F38&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="19">
+        <v>193013038</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="26">
+        <f>VLOOKUP(A39,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D39" s="26">
+        <f>VLOOKUP(A39,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E39" s="27">
+        <f>C39+D39</f>
+        <v>12</v>
+      </c>
+      <c r="F39" s="24">
+        <f>(E39/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G39" s="18" t="str">
+        <f>IF(F39&gt;94,"A+",IF(F39&gt;84,"A",IF(F39&gt;79,"A-",IF(F39&gt;74,"B+",IF(F39&gt;69,"B",IF(F39&gt;64,"B-",IF(F39&gt;59,"C+",IF(F39&gt;54,"C",IF(F39&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="19">
+        <v>193013043</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="26">
+        <f>VLOOKUP(A40,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="26">
+        <f>VLOOKUP(A40,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E40" s="27">
+        <f>C40+D40</f>
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <f>(E40/E$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="G40" s="18" t="str">
+        <f>IF(F40&gt;94,"A+",IF(F40&gt;84,"A",IF(F40&gt;79,"A-",IF(F40&gt;74,"B+",IF(F40&gt;69,"B",IF(F40&gt;64,"B-",IF(F40&gt;59,"C+",IF(F40&gt;54,"C",IF(F40&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="19">
+        <v>193013046</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="26">
+        <f>VLOOKUP(A41,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D41" s="26">
+        <f>VLOOKUP(A41,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E41" s="27">
+        <f>C41+D41</f>
+        <v>11.5</v>
+      </c>
+      <c r="F41" s="24">
+        <f>(E41/E$50)*100</f>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="G41" s="18" t="str">
+        <f>IF(F41&gt;94,"A+",IF(F41&gt;84,"A",IF(F41&gt;79,"A-",IF(F41&gt;74,"B+",IF(F41&gt;69,"B",IF(F41&gt;64,"B-",IF(F41&gt;59,"C+",IF(F41&gt;54,"C",IF(F41&gt;49,"D","F")))))))))</f>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="19">
+        <v>193013050</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="26">
+        <f>VLOOKUP(A42,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="26">
+        <f>VLOOKUP(A42,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" s="27">
+        <f>C42+D42</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="24">
+        <f>(E42/E$50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="18" t="str">
+        <f>IF(F42&gt;94,"A+",IF(F42&gt;84,"A",IF(F42&gt;79,"A-",IF(F42&gt;74,"B+",IF(F42&gt;69,"B",IF(F42&gt;64,"B-",IF(F42&gt;59,"C+",IF(F42&gt;54,"C",IF(F42&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="19">
+        <v>193013055</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="26">
+        <f>VLOOKUP(A43,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="26">
+        <f>VLOOKUP(A43,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E43" s="27">
+        <f>C43+D43</f>
+        <v>9</v>
+      </c>
+      <c r="F43" s="24">
+        <f>(E43/E$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="G43" s="18" t="str">
+        <f>IF(F43&gt;94,"A+",IF(F43&gt;84,"A",IF(F43&gt;79,"A-",IF(F43&gt;74,"B+",IF(F43&gt;69,"B",IF(F43&gt;64,"B-",IF(F43&gt;59,"C+",IF(F43&gt;54,"C",IF(F43&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
+        <v>193013088</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="26">
+        <f>VLOOKUP(A44,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D44" s="26">
+        <f>VLOOKUP(A44,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E44" s="27">
+        <f>C44+D44</f>
+        <v>12</v>
+      </c>
+      <c r="F44" s="24">
+        <f>(E44/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G44" s="18" t="str">
+        <f>IF(F44&gt;94,"A+",IF(F44&gt;84,"A",IF(F44&gt;79,"A-",IF(F44&gt;74,"B+",IF(F44&gt;69,"B",IF(F44&gt;64,"B-",IF(F44&gt;59,"C+",IF(F44&gt;54,"C",IF(F44&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="19">
+        <v>193013096</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="26">
+        <f>VLOOKUP(A45,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D45" s="26">
+        <f>VLOOKUP(A45,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E45" s="27">
+        <f>C45+D45</f>
+        <v>12.5</v>
+      </c>
+      <c r="F45" s="24">
+        <f>(E45/E$50)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="G45" s="18" t="str">
+        <f>IF(F45&gt;94,"A+",IF(F45&gt;84,"A",IF(F45&gt;79,"A-",IF(F45&gt;74,"B+",IF(F45&gt;69,"B",IF(F45&gt;64,"B-",IF(F45&gt;59,"C+",IF(F45&gt;54,"C",IF(F45&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="19">
+        <v>182014039</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="26">
+        <f>VLOOKUP(A46,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D46" s="26">
+        <f>VLOOKUP(A46,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E46" s="27">
+        <f>C46+D46</f>
+        <v>9</v>
+      </c>
+      <c r="F46" s="24">
+        <f>(E46/E$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="G46" s="18" t="str">
+        <f>IF(F46&gt;94,"A+",IF(F46&gt;84,"A",IF(F46&gt;79,"A-",IF(F46&gt;74,"B+",IF(F46&gt;69,"B",IF(F46&gt;64,"B-",IF(F46&gt;59,"C+",IF(F46&gt;54,"C",IF(F46&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="19">
+        <v>183016004</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="26">
+        <f>VLOOKUP(A47,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D47" s="26">
+        <f>VLOOKUP(A47,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E47" s="27">
+        <f>C47+D47</f>
+        <v>14</v>
+      </c>
+      <c r="F47" s="24">
+        <f>(E47/E$50)*100</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="G47" s="18" t="str">
+        <f>IF(F47&gt;94,"A+",IF(F47&gt;84,"A",IF(F47&gt;79,"A-",IF(F47&gt;74,"B+",IF(F47&gt;69,"B",IF(F47&gt;64,"B-",IF(F47&gt;59,"C+",IF(F47&gt;54,"C",IF(F47&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="19">
+        <v>193016002</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="26">
+        <f>VLOOKUP(A48,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D48" s="26">
+        <f>VLOOKUP(A48,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E48" s="27">
+        <f>C48+D48</f>
+        <v>11</v>
+      </c>
+      <c r="F48" s="24">
+        <f>(E48/E$50)*100</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="G48" s="18" t="str">
+        <f>IF(F48&gt;94,"A+",IF(F48&gt;84,"A",IF(F48&gt;79,"A-",IF(F48&gt;74,"B+",IF(F48&gt;69,"B",IF(F48&gt;64,"B-",IF(F48&gt;59,"C+",IF(F48&gt;54,"C",IF(F48&gt;49,"D","F")))))))))</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="17">
+        <v>193016004</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="15">
+        <f>VLOOKUP(A49,[1]Sheet1!B$2:C$55,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D49" s="15">
+        <f>VLOOKUP(A49,[1]Sheet1!D$2:E$55,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E49" s="14">
+        <f>C49+D49</f>
+        <v>12</v>
+      </c>
+      <c r="F49" s="13">
+        <f>(E49/E$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="G49" s="12" t="str">
+        <f>IF(F49&gt;94,"A+",IF(F49&gt;84,"A",IF(F49&gt;79,"A-",IF(F49&gt;74,"B+",IF(F49&gt;69,"B",IF(F49&gt;64,"B-",IF(F49&gt;59,"C+",IF(F49&gt;54,"C",IF(F49&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="10">
+        <v>5</v>
+      </c>
+      <c r="D50" s="10">
+        <v>10</v>
+      </c>
+      <c r="E50" s="11">
+        <f>C50+D50</f>
+        <v>15</v>
+      </c>
+      <c r="F50" s="24">
+        <f>(E50/E$50)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added attendance for cse 101 section 8
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101 Non CSE/results_cse101_sec8.xlsx
+++ b/FALL 19/CSE 101 Non CSE/results_cse101_sec8.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\CSE 101 Non CSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E775CC4-FDEA-4306-A6DD-02C5BA648DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C20C74-955F-4234-8C64-56F0A18E8D10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="quiz1" sheetId="1" r:id="rId1"/>
-    <sheet name="mid1" sheetId="2" r:id="rId2"/>
-    <sheet name="mid2" sheetId="3" r:id="rId3"/>
-    <sheet name="mid_total" sheetId="4" r:id="rId4"/>
-    <sheet name="final" sheetId="5" r:id="rId5"/>
-    <sheet name="presentation" sheetId="6" r:id="rId6"/>
+    <sheet name="attendance" sheetId="7" r:id="rId1"/>
+    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
+    <sheet name="mid1" sheetId="2" r:id="rId3"/>
+    <sheet name="mid2" sheetId="3" r:id="rId4"/>
+    <sheet name="mid_total" sheetId="4" r:id="rId5"/>
+    <sheet name="final" sheetId="5" r:id="rId6"/>
+    <sheet name="presentation" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -253,12 +254,18 @@
   <si>
     <t>Presentation</t>
   </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,6 +313,12 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -474,12 +487,69 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D52BF41C-157E-415A-A241-C642C3EFA20F}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -733,6 +803,7 @@
           <cell r="B8">
             <v>192011003</v>
           </cell>
+          <cell r="C8"/>
           <cell r="D8">
             <v>192011003</v>
           </cell>
@@ -898,6 +969,7 @@
           <cell r="D25">
             <v>193013005</v>
           </cell>
+          <cell r="E25"/>
         </row>
         <row r="27">
           <cell r="B27">
@@ -1436,14 +1508,1515 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE00863-EDCE-4A2D-A663-7BB94F862ACC}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="8" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="33">
+        <v>191011023</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="35">
+        <v>19</v>
+      </c>
+      <c r="D2" s="35">
+        <v>5</v>
+      </c>
+      <c r="E2" s="35">
+        <f>C2-D2</f>
+        <v>14</v>
+      </c>
+      <c r="F2" s="35">
+        <f>ROUNDUP((E2/C2)*F$50,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G2" s="36">
+        <f>(F2/F$50)*100</f>
+        <v>80</v>
+      </c>
+      <c r="H2" s="32" t="str">
+        <f>IF(G2&gt;94,"A+",IF(G2&gt;84,"A",IF(G2&gt;79,"A-",IF(G2&gt;74,"B+",IF(G2&gt;69,"B",IF(G2&gt;64,"B-",IF(G2&gt;59,"C+",IF(G2&gt;54,"C",IF(G2&gt;49,"D","F")))))))))</f>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="33">
+        <v>191011053</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="37">
+        <v>16</v>
+      </c>
+      <c r="D3" s="37">
+        <v>7</v>
+      </c>
+      <c r="E3" s="35">
+        <f t="shared" ref="E3:E49" si="0">C3-D3</f>
+        <v>9</v>
+      </c>
+      <c r="F3" s="35">
+        <f t="shared" ref="F3:F49" si="1">ROUNDUP((E3/C3)*F$50,0)</f>
+        <v>6</v>
+      </c>
+      <c r="G3" s="36">
+        <f t="shared" ref="G3:G49" si="2">(F3/F$50)*100</f>
+        <v>60</v>
+      </c>
+      <c r="H3" s="32" t="str">
+        <f t="shared" ref="H3:H49" si="3">IF(G3&gt;94,"A+",IF(G3&gt;84,"A",IF(G3&gt;79,"A-",IF(G3&gt;74,"B+",IF(G3&gt;69,"B",IF(G3&gt;64,"B-",IF(G3&gt;59,"C+",IF(G3&gt;54,"C",IF(G3&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="33">
+        <v>191011226</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="37">
+        <v>19</v>
+      </c>
+      <c r="D4" s="37">
+        <v>7</v>
+      </c>
+      <c r="E4" s="35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G4" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H4" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="33">
+        <v>192011003</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="37">
+        <v>16</v>
+      </c>
+      <c r="D5" s="37">
+        <v>15</v>
+      </c>
+      <c r="E5" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="36">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="33">
+        <v>192011051</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="44">
+        <v>17</v>
+      </c>
+      <c r="D6" s="44">
+        <v>2</v>
+      </c>
+      <c r="E6" s="35">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G6" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H6" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="33">
+        <v>192011116</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="44">
+        <v>17</v>
+      </c>
+      <c r="D7" s="44">
+        <v>7</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="36">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H7" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
+        <v>192011156</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="44">
+        <v>16</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0</v>
+      </c>
+      <c r="E8" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F8" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H8" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="33">
+        <v>193011005</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="44">
+        <v>19</v>
+      </c>
+      <c r="D9" s="44">
+        <v>3</v>
+      </c>
+      <c r="E9" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G9" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H9" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>193011025</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="44">
+        <v>19</v>
+      </c>
+      <c r="D10" s="44">
+        <v>1</v>
+      </c>
+      <c r="E10" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F10" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H10" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="33">
+        <v>193011035</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="44">
+        <v>19</v>
+      </c>
+      <c r="D11" s="44">
+        <v>6</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F11" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H11" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>193011069</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="44">
+        <v>19</v>
+      </c>
+      <c r="D12" s="44">
+        <v>3</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F12" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H12" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
+        <v>193011075</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="44">
+        <v>19</v>
+      </c>
+      <c r="D13" s="44">
+        <v>1</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F13" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H13" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>193011105</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="44">
+        <v>15</v>
+      </c>
+      <c r="D14" s="44">
+        <v>10</v>
+      </c>
+      <c r="E14" s="35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="36">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="33">
+        <v>193011116</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="44">
+        <v>19</v>
+      </c>
+      <c r="D15" s="44">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F15" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H15" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="33">
+        <v>193011117</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="44">
+        <v>19</v>
+      </c>
+      <c r="D16" s="44">
+        <v>3</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F16" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H16" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="33">
+        <v>193011122</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="44">
+        <v>19</v>
+      </c>
+      <c r="D17" s="44">
+        <v>5</v>
+      </c>
+      <c r="E17" s="35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F17" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G17" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H17" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
+        <v>193011123</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="44">
+        <v>19</v>
+      </c>
+      <c r="D18" s="44">
+        <v>1</v>
+      </c>
+      <c r="E18" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F18" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H18" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="33">
+        <v>193011128</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="44">
+        <v>19</v>
+      </c>
+      <c r="D19" s="44">
+        <v>13</v>
+      </c>
+      <c r="E19" s="35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G19" s="36">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H19" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="33">
+        <v>193011133</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="44">
+        <v>19</v>
+      </c>
+      <c r="D20" s="44">
+        <v>3</v>
+      </c>
+      <c r="E20" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F20" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G20" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H20" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="33">
+        <v>193011152</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="44">
+        <v>19</v>
+      </c>
+      <c r="D21" s="44">
+        <v>2</v>
+      </c>
+      <c r="E21" s="35">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F21" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G21" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H21" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="33">
+        <v>193011166</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="44">
+        <v>19</v>
+      </c>
+      <c r="D22" s="44">
+        <v>1</v>
+      </c>
+      <c r="E22" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F22" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G22" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H22" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="33">
+        <v>193011176</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="44">
+        <v>19</v>
+      </c>
+      <c r="D23" s="44">
+        <v>8</v>
+      </c>
+      <c r="E23" s="35">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F23" s="35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G23" s="36">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H23" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="33">
+        <v>193011181</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="44">
+        <v>19</v>
+      </c>
+      <c r="D24" s="44">
+        <v>6</v>
+      </c>
+      <c r="E24" s="35">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F24" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G24" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H24" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="33">
+        <v>193011185</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="44">
+        <v>19</v>
+      </c>
+      <c r="D25" s="44">
+        <v>5</v>
+      </c>
+      <c r="E25" s="35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F25" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G25" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H25" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="33">
+        <v>193011189</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="44">
+        <v>19</v>
+      </c>
+      <c r="D26" s="44">
+        <v>5</v>
+      </c>
+      <c r="E26" s="35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F26" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G26" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H26" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="33">
+        <v>193011194</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="44">
+        <v>19</v>
+      </c>
+      <c r="D27" s="44">
+        <v>1</v>
+      </c>
+      <c r="E27" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F27" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G27" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H27" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="33">
+        <v>191012011</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="37">
+        <v>19</v>
+      </c>
+      <c r="D28" s="37">
+        <v>1</v>
+      </c>
+      <c r="E28" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F28" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G28" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H28" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="33">
+        <v>191012060</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="37">
+        <v>19</v>
+      </c>
+      <c r="D29" s="37">
+        <v>6</v>
+      </c>
+      <c r="E29" s="35">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F29" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G29" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H29" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="33">
+        <v>191012061</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="37">
+        <v>19</v>
+      </c>
+      <c r="D30" s="37">
+        <v>13</v>
+      </c>
+      <c r="E30" s="35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F30" s="35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G30" s="36">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H30" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="33">
+        <v>173013015</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="37">
+        <v>17</v>
+      </c>
+      <c r="D31" s="37">
+        <v>6</v>
+      </c>
+      <c r="E31" s="35">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F31" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G31" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H31" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="33">
+        <v>182013026</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="37">
+        <v>15</v>
+      </c>
+      <c r="D32" s="37">
+        <v>7</v>
+      </c>
+      <c r="E32" s="35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F32" s="35">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G32" s="36">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H32" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="33">
+        <v>193013005</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="44">
+        <v>19</v>
+      </c>
+      <c r="D33" s="44">
+        <v>10</v>
+      </c>
+      <c r="E33" s="35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F33" s="35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G33" s="36">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H33" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="33">
+        <v>193013006</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="44">
+        <v>19</v>
+      </c>
+      <c r="D34" s="44">
+        <v>2</v>
+      </c>
+      <c r="E34" s="35">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F34" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G34" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H34" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="33">
+        <v>193013008</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="44">
+        <v>19</v>
+      </c>
+      <c r="D35" s="44">
+        <v>0</v>
+      </c>
+      <c r="E35" s="35">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F35" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G35" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H35" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="33">
+        <v>193013015</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="44">
+        <v>19</v>
+      </c>
+      <c r="D36" s="44">
+        <v>3</v>
+      </c>
+      <c r="E36" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F36" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G36" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H36" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="33">
+        <v>193013021</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="44">
+        <v>19</v>
+      </c>
+      <c r="D37" s="44">
+        <v>0</v>
+      </c>
+      <c r="E37" s="35">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F37" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G37" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H37" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="33">
+        <v>193013030</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="44">
+        <v>19</v>
+      </c>
+      <c r="D38" s="44">
+        <v>3</v>
+      </c>
+      <c r="E38" s="35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F38" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G38" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H38" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="33">
+        <v>193013038</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="44">
+        <v>19</v>
+      </c>
+      <c r="D39" s="44">
+        <v>1</v>
+      </c>
+      <c r="E39" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F39" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G39" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H39" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="33">
+        <v>193013043</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="44">
+        <v>19</v>
+      </c>
+      <c r="D40" s="44">
+        <v>11</v>
+      </c>
+      <c r="E40" s="35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F40" s="35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="36">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H40" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="33">
+        <v>193013046</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="44">
+        <v>19</v>
+      </c>
+      <c r="D41" s="44">
+        <v>5</v>
+      </c>
+      <c r="E41" s="35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F41" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G41" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H41" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="33">
+        <v>193013050</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="44">
+        <v>19</v>
+      </c>
+      <c r="D42" s="44">
+        <v>7</v>
+      </c>
+      <c r="E42" s="35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F42" s="35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="36">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H42" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="33">
+        <v>193013055</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="44">
+        <v>19</v>
+      </c>
+      <c r="D43" s="44">
+        <v>17</v>
+      </c>
+      <c r="E43" s="35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F43" s="35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G43" s="36">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H43" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="33">
+        <v>193013088</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="44">
+        <v>19</v>
+      </c>
+      <c r="D44" s="44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="35">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F44" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G44" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H44" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="33">
+        <v>193013096</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="44">
+        <v>16</v>
+      </c>
+      <c r="D45" s="44">
+        <v>4</v>
+      </c>
+      <c r="E45" s="35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F45" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G45" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H45" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="33">
+        <v>182014039</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="44">
+        <v>16</v>
+      </c>
+      <c r="D46" s="44">
+        <v>1</v>
+      </c>
+      <c r="E46" s="35">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F46" s="35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G46" s="36">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H46" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="33">
+        <v>183016004</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="37">
+        <v>18</v>
+      </c>
+      <c r="D47" s="37">
+        <v>3</v>
+      </c>
+      <c r="E47" s="35">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F47" s="35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G47" s="36">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H47" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="33">
+        <v>193016002</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="44">
+        <v>19</v>
+      </c>
+      <c r="D48" s="44">
+        <v>5</v>
+      </c>
+      <c r="E48" s="35">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F48" s="35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G48" s="36">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H48" s="32" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="38">
+        <v>193016004</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="40">
+        <v>19</v>
+      </c>
+      <c r="D49" s="40">
+        <v>2</v>
+      </c>
+      <c r="E49" s="41">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F49" s="41">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G49" s="42">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H49" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="F50" s="31">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:E2 E3:E49">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H49">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3478,17 +5051,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C49">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E49">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G49">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3497,7 +5070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
@@ -5748,22 +7321,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C49">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E49">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G49">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I49">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5772,7 +7345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82CC3F2-F78F-4F4B-8DA0-5BBD0E38DEE9}">
   <dimension ref="A1:N49"/>
   <sheetViews>
@@ -7847,22 +9420,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C49">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E49">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G49">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I49">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7870,7 +9443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F18057-465E-4691-A948-5DA6A053A16C}">
   <dimension ref="A1:I49"/>
   <sheetViews>
@@ -9504,7 +11077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355CD6C3-0968-416E-AD99-DA1E04F24285}">
   <dimension ref="A1:R49"/>
   <sheetViews>
@@ -12262,22 +13835,22 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C2:C49">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E49">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G49">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12285,11 +13858,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36981321-2A1A-46DA-A7F6-4FDFF056C86A}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -12340,15 +13913,15 @@
         <v>6</v>
       </c>
       <c r="E2" s="27">
-        <f>C2+D2</f>
+        <f t="shared" ref="E2:E33" si="0">C2+D2</f>
         <v>9</v>
       </c>
       <c r="F2" s="24">
-        <f>(E2/E$50)*100</f>
+        <f t="shared" ref="F2:F33" si="1">(E2/E$50)*100</f>
         <v>60</v>
       </c>
       <c r="G2" s="18" t="str">
-        <f>IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="G2:G49" si="2">IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
         <v>C+</v>
       </c>
     </row>
@@ -12368,15 +13941,15 @@
         <v>8.5</v>
       </c>
       <c r="E3" s="27">
-        <f>C3+D3</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="F3" s="24">
-        <f>(E3/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>56.666666666666664</v>
       </c>
       <c r="G3" s="18" t="str">
-        <f>IF(F3&gt;94,"A+",IF(F3&gt;84,"A",IF(F3&gt;79,"A-",IF(F3&gt;74,"B+",IF(F3&gt;69,"B",IF(F3&gt;64,"B-",IF(F3&gt;59,"C+",IF(F3&gt;54,"C",IF(F3&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -12396,15 +13969,15 @@
         <v>6</v>
       </c>
       <c r="E4" s="27">
-        <f>C4+D4</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="F4" s="24">
-        <f>(E4/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>56.666666666666664</v>
       </c>
       <c r="G4" s="18" t="str">
-        <f>IF(F4&gt;94,"A+",IF(F4&gt;84,"A",IF(F4&gt;79,"A-",IF(F4&gt;74,"B+",IF(F4&gt;69,"B",IF(F4&gt;64,"B-",IF(F4&gt;59,"C+",IF(F4&gt;54,"C",IF(F4&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -12424,15 +13997,15 @@
         <v>8</v>
       </c>
       <c r="E5" s="27">
-        <f>C5+D5</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F5" s="24">
-        <f>(E5/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>53.333333333333336</v>
       </c>
       <c r="G5" s="18" t="str">
-        <f>IF(F5&gt;94,"A+",IF(F5&gt;84,"A",IF(F5&gt;79,"A-",IF(F5&gt;74,"B+",IF(F5&gt;69,"B",IF(F5&gt;64,"B-",IF(F5&gt;59,"C+",IF(F5&gt;54,"C",IF(F5&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
     </row>
@@ -12452,15 +14025,15 @@
         <v>6</v>
       </c>
       <c r="E6" s="27">
-        <f>C6+D6</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="F6" s="24">
-        <f>(E6/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>56.666666666666664</v>
       </c>
       <c r="G6" s="18" t="str">
-        <f>IF(F6&gt;94,"A+",IF(F6&gt;84,"A",IF(F6&gt;79,"A-",IF(F6&gt;74,"B+",IF(F6&gt;69,"B",IF(F6&gt;64,"B-",IF(F6&gt;59,"C+",IF(F6&gt;54,"C",IF(F6&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -12480,15 +14053,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="27">
-        <f>C7+D7</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F7" s="24">
-        <f>(E7/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="G7" s="18" t="str">
-        <f>IF(F7&gt;94,"A+",IF(F7&gt;84,"A",IF(F7&gt;79,"A-",IF(F7&gt;74,"B+",IF(F7&gt;69,"B",IF(F7&gt;64,"B-",IF(F7&gt;59,"C+",IF(F7&gt;54,"C",IF(F7&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
@@ -12508,15 +14081,15 @@
         <v>8</v>
       </c>
       <c r="E8" s="27">
-        <f>C8+D8</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F8" s="24">
-        <f>(E8/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G8" s="18" t="str">
-        <f>IF(F8&gt;94,"A+",IF(F8&gt;84,"A",IF(F8&gt;79,"A-",IF(F8&gt;74,"B+",IF(F8&gt;69,"B",IF(F8&gt;64,"B-",IF(F8&gt;59,"C+",IF(F8&gt;54,"C",IF(F8&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -12536,15 +14109,15 @@
         <v>8.5</v>
       </c>
       <c r="E9" s="27">
-        <f>C9+D9</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="F9" s="24">
-        <f>(E9/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>76.666666666666671</v>
       </c>
       <c r="G9" s="18" t="str">
-        <f>IF(F9&gt;94,"A+",IF(F9&gt;84,"A",IF(F9&gt;79,"A-",IF(F9&gt;74,"B+",IF(F9&gt;69,"B",IF(F9&gt;64,"B-",IF(F9&gt;59,"C+",IF(F9&gt;54,"C",IF(F9&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B+</v>
       </c>
     </row>
@@ -12564,15 +14137,15 @@
         <v>8.5</v>
       </c>
       <c r="E10" s="27">
-        <f>C10+D10</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F10" s="24">
-        <f>(E10/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>86.666666666666671</v>
       </c>
       <c r="G10" s="18" t="str">
-        <f>IF(F10&gt;94,"A+",IF(F10&gt;84,"A",IF(F10&gt;79,"A-",IF(F10&gt;74,"B+",IF(F10&gt;69,"B",IF(F10&gt;64,"B-",IF(F10&gt;59,"C+",IF(F10&gt;54,"C",IF(F10&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -12592,15 +14165,15 @@
         <v>8</v>
       </c>
       <c r="E11" s="27">
-        <f>C11+D11</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F11" s="24">
-        <f>(E11/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G11" s="18" t="str">
-        <f>IF(F11&gt;94,"A+",IF(F11&gt;84,"A",IF(F11&gt;79,"A-",IF(F11&gt;74,"B+",IF(F11&gt;69,"B",IF(F11&gt;64,"B-",IF(F11&gt;59,"C+",IF(F11&gt;54,"C",IF(F11&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -12620,15 +14193,15 @@
         <v>6</v>
       </c>
       <c r="E12" s="27">
-        <f>C12+D12</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="F12" s="24">
-        <f>(E12/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>63.333333333333329</v>
       </c>
       <c r="G12" s="18" t="str">
-        <f>IF(F12&gt;94,"A+",IF(F12&gt;84,"A",IF(F12&gt;79,"A-",IF(F12&gt;74,"B+",IF(F12&gt;69,"B",IF(F12&gt;64,"B-",IF(F12&gt;59,"C+",IF(F12&gt;54,"C",IF(F12&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
@@ -12648,15 +14221,15 @@
         <v>8.5</v>
       </c>
       <c r="E13" s="27">
-        <f>C13+D13</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="F13" s="24">
-        <f>(E13/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="G13" s="18" t="str">
-        <f>IF(F13&gt;94,"A+",IF(F13&gt;84,"A",IF(F13&gt;79,"A-",IF(F13&gt;74,"B+",IF(F13&gt;69,"B",IF(F13&gt;64,"B-",IF(F13&gt;59,"C+",IF(F13&gt;54,"C",IF(F13&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -12676,15 +14249,15 @@
         <v>0</v>
       </c>
       <c r="E14" s="27">
-        <f>C14+D14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="24">
-        <f>(E14/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14" s="18" t="str">
-        <f>IF(F14&gt;94,"A+",IF(F14&gt;84,"A",IF(F14&gt;79,"A-",IF(F14&gt;74,"B+",IF(F14&gt;69,"B",IF(F14&gt;64,"B-",IF(F14&gt;59,"C+",IF(F14&gt;54,"C",IF(F14&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -12704,15 +14277,15 @@
         <v>9</v>
       </c>
       <c r="E15" s="27">
-        <f>C15+D15</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F15" s="24">
-        <f>(E15/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G15" s="18" t="str">
-        <f>IF(F15&gt;94,"A+",IF(F15&gt;84,"A",IF(F15&gt;79,"A-",IF(F15&gt;74,"B+",IF(F15&gt;69,"B",IF(F15&gt;64,"B-",IF(F15&gt;59,"C+",IF(F15&gt;54,"C",IF(F15&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -12732,15 +14305,15 @@
         <v>0</v>
       </c>
       <c r="E16" s="27">
-        <f>C16+D16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" s="24">
-        <f>(E16/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="18" t="str">
-        <f>IF(F16&gt;94,"A+",IF(F16&gt;84,"A",IF(F16&gt;79,"A-",IF(F16&gt;74,"B+",IF(F16&gt;69,"B",IF(F16&gt;64,"B-",IF(F16&gt;59,"C+",IF(F16&gt;54,"C",IF(F16&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -12760,15 +14333,15 @@
         <v>8.5</v>
       </c>
       <c r="E17" s="27">
-        <f>C17+D17</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F17" s="24">
-        <f>(E17/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>73.333333333333329</v>
       </c>
       <c r="G17" s="18" t="str">
-        <f>IF(F17&gt;94,"A+",IF(F17&gt;84,"A",IF(F17&gt;79,"A-",IF(F17&gt;74,"B+",IF(F17&gt;69,"B",IF(F17&gt;64,"B-",IF(F17&gt;59,"C+",IF(F17&gt;54,"C",IF(F17&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -12788,15 +14361,15 @@
         <v>8.5</v>
       </c>
       <c r="E18" s="27">
-        <f>C18+D18</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F18" s="24">
-        <f>(E18/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>73.333333333333329</v>
       </c>
       <c r="G18" s="18" t="str">
-        <f>IF(F18&gt;94,"A+",IF(F18&gt;84,"A",IF(F18&gt;79,"A-",IF(F18&gt;74,"B+",IF(F18&gt;69,"B",IF(F18&gt;64,"B-",IF(F18&gt;59,"C+",IF(F18&gt;54,"C",IF(F18&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -12816,15 +14389,15 @@
         <v>6</v>
       </c>
       <c r="E19" s="27">
-        <f>C19+D19</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F19" s="24">
-        <f>(E19/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G19" s="18" t="str">
-        <f>IF(F19&gt;94,"A+",IF(F19&gt;84,"A",IF(F19&gt;79,"A-",IF(F19&gt;74,"B+",IF(F19&gt;69,"B",IF(F19&gt;64,"B-",IF(F19&gt;59,"C+",IF(F19&gt;54,"C",IF(F19&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -12844,15 +14417,15 @@
         <v>6</v>
       </c>
       <c r="E20" s="27">
-        <f>C20+D20</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="F20" s="24">
-        <f>(E20/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>56.666666666666664</v>
       </c>
       <c r="G20" s="18" t="str">
-        <f>IF(F20&gt;94,"A+",IF(F20&gt;84,"A",IF(F20&gt;79,"A-",IF(F20&gt;74,"B+",IF(F20&gt;69,"B",IF(F20&gt;64,"B-",IF(F20&gt;59,"C+",IF(F20&gt;54,"C",IF(F20&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
@@ -12872,15 +14445,15 @@
         <v>8.5</v>
       </c>
       <c r="E21" s="27">
-        <f>C21+D21</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F21" s="24">
-        <f>(E21/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>73.333333333333329</v>
       </c>
       <c r="G21" s="18" t="str">
-        <f>IF(F21&gt;94,"A+",IF(F21&gt;84,"A",IF(F21&gt;79,"A-",IF(F21&gt;74,"B+",IF(F21&gt;69,"B",IF(F21&gt;64,"B-",IF(F21&gt;59,"C+",IF(F21&gt;54,"C",IF(F21&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -12900,15 +14473,15 @@
         <v>8</v>
       </c>
       <c r="E22" s="27">
-        <f>C22+D22</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="F22" s="24">
-        <f>(E22/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>76.666666666666671</v>
       </c>
       <c r="G22" s="18" t="str">
-        <f>IF(F22&gt;94,"A+",IF(F22&gt;84,"A",IF(F22&gt;79,"A-",IF(F22&gt;74,"B+",IF(F22&gt;69,"B",IF(F22&gt;64,"B-",IF(F22&gt;59,"C+",IF(F22&gt;54,"C",IF(F22&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B+</v>
       </c>
     </row>
@@ -12928,15 +14501,15 @@
         <v>0</v>
       </c>
       <c r="E23" s="27">
-        <f>C23+D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="24">
-        <f>(E23/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G23" s="18" t="str">
-        <f>IF(F23&gt;94,"A+",IF(F23&gt;84,"A",IF(F23&gt;79,"A-",IF(F23&gt;74,"B+",IF(F23&gt;69,"B",IF(F23&gt;64,"B-",IF(F23&gt;59,"C+",IF(F23&gt;54,"C",IF(F23&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -12956,15 +14529,15 @@
         <v>8</v>
       </c>
       <c r="E24" s="27">
-        <f>C24+D24</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F24" s="24">
-        <f>(E24/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G24" s="18" t="str">
-        <f>IF(F24&gt;94,"A+",IF(F24&gt;84,"A",IF(F24&gt;79,"A-",IF(F24&gt;74,"B+",IF(F24&gt;69,"B",IF(F24&gt;64,"B-",IF(F24&gt;59,"C+",IF(F24&gt;54,"C",IF(F24&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -12984,15 +14557,15 @@
         <v>0</v>
       </c>
       <c r="E25" s="27">
-        <f>C25+D25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25" s="24">
-        <f>(E25/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="18" t="str">
-        <f>IF(F25&gt;94,"A+",IF(F25&gt;84,"A",IF(F25&gt;79,"A-",IF(F25&gt;74,"B+",IF(F25&gt;69,"B",IF(F25&gt;64,"B-",IF(F25&gt;59,"C+",IF(F25&gt;54,"C",IF(F25&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13012,15 +14585,15 @@
         <v>8</v>
       </c>
       <c r="E26" s="27">
-        <f>C26+D26</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F26" s="24">
-        <f>(E26/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="G26" s="18" t="str">
-        <f>IF(F26&gt;94,"A+",IF(F26&gt;84,"A",IF(F26&gt;79,"A-",IF(F26&gt;74,"B+",IF(F26&gt;69,"B",IF(F26&gt;64,"B-",IF(F26&gt;59,"C+",IF(F26&gt;54,"C",IF(F26&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13040,15 +14613,15 @@
         <v>0</v>
       </c>
       <c r="E27" s="27">
-        <f>C27+D27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="24">
-        <f>(E27/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="18" t="str">
-        <f>IF(F27&gt;94,"A+",IF(F27&gt;84,"A",IF(F27&gt;79,"A-",IF(F27&gt;74,"B+",IF(F27&gt;69,"B",IF(F27&gt;64,"B-",IF(F27&gt;59,"C+",IF(F27&gt;54,"C",IF(F27&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13068,15 +14641,15 @@
         <v>8</v>
       </c>
       <c r="E28" s="27">
-        <f>C28+D28</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" s="24">
-        <f>(E28/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>53.333333333333336</v>
       </c>
       <c r="G28" s="18" t="str">
-        <f>IF(F28&gt;94,"A+",IF(F28&gt;84,"A",IF(F28&gt;79,"A-",IF(F28&gt;74,"B+",IF(F28&gt;69,"B",IF(F28&gt;64,"B-",IF(F28&gt;59,"C+",IF(F28&gt;54,"C",IF(F28&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
     </row>
@@ -13096,15 +14669,15 @@
         <v>0</v>
       </c>
       <c r="E29" s="27">
-        <f>C29+D29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29" s="24">
-        <f>(E29/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29" s="18" t="str">
-        <f>IF(F29&gt;94,"A+",IF(F29&gt;84,"A",IF(F29&gt;79,"A-",IF(F29&gt;74,"B+",IF(F29&gt;69,"B",IF(F29&gt;64,"B-",IF(F29&gt;59,"C+",IF(F29&gt;54,"C",IF(F29&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13124,15 +14697,15 @@
         <v>6</v>
       </c>
       <c r="E30" s="27">
-        <f>C30+D30</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F30" s="24">
-        <f>(E30/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G30" s="18" t="str">
-        <f>IF(F30&gt;94,"A+",IF(F30&gt;84,"A",IF(F30&gt;79,"A-",IF(F30&gt;74,"B+",IF(F30&gt;69,"B",IF(F30&gt;64,"B-",IF(F30&gt;59,"C+",IF(F30&gt;54,"C",IF(F30&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13152,15 +14725,15 @@
         <v>0</v>
       </c>
       <c r="E31" s="27">
-        <f>C31+D31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="24">
-        <f>(E31/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31" s="18" t="str">
-        <f>IF(F31&gt;94,"A+",IF(F31&gt;84,"A",IF(F31&gt;79,"A-",IF(F31&gt;74,"B+",IF(F31&gt;69,"B",IF(F31&gt;64,"B-",IF(F31&gt;59,"C+",IF(F31&gt;54,"C",IF(F31&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13180,15 +14753,15 @@
         <v>8</v>
       </c>
       <c r="E32" s="27">
-        <f>C32+D32</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F32" s="24">
-        <f>(E32/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>53.333333333333336</v>
       </c>
       <c r="G32" s="18" t="str">
-        <f>IF(F32&gt;94,"A+",IF(F32&gt;84,"A",IF(F32&gt;79,"A-",IF(F32&gt;74,"B+",IF(F32&gt;69,"B",IF(F32&gt;64,"B-",IF(F32&gt;59,"C+",IF(F32&gt;54,"C",IF(F32&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
     </row>
@@ -13208,15 +14781,15 @@
         <v>0</v>
       </c>
       <c r="E33" s="27">
-        <f>C33+D33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F33" s="24">
-        <f>(E33/E$50)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G33" s="18" t="str">
-        <f>IF(F33&gt;94,"A+",IF(F33&gt;84,"A",IF(F33&gt;79,"A-",IF(F33&gt;74,"B+",IF(F33&gt;69,"B",IF(F33&gt;64,"B-",IF(F33&gt;59,"C+",IF(F33&gt;54,"C",IF(F33&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13236,15 +14809,15 @@
         <v>0</v>
       </c>
       <c r="E34" s="27">
-        <f>C34+D34</f>
+        <f t="shared" ref="E34:E65" si="3">C34+D34</f>
         <v>0</v>
       </c>
       <c r="F34" s="24">
-        <f>(E34/E$50)*100</f>
+        <f t="shared" ref="F34:F65" si="4">(E34/E$50)*100</f>
         <v>0</v>
       </c>
       <c r="G34" s="18" t="str">
-        <f>IF(F34&gt;94,"A+",IF(F34&gt;84,"A",IF(F34&gt;79,"A-",IF(F34&gt;74,"B+",IF(F34&gt;69,"B",IF(F34&gt;64,"B-",IF(F34&gt;59,"C+",IF(F34&gt;54,"C",IF(F34&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13264,15 +14837,15 @@
         <v>8</v>
       </c>
       <c r="E35" s="27">
-        <f>C35+D35</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="F35" s="24">
-        <f>(E35/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="G35" s="18" t="str">
-        <f>IF(F35&gt;94,"A+",IF(F35&gt;84,"A",IF(F35&gt;79,"A-",IF(F35&gt;74,"B+",IF(F35&gt;69,"B",IF(F35&gt;64,"B-",IF(F35&gt;59,"C+",IF(F35&gt;54,"C",IF(F35&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13292,15 +14865,15 @@
         <v>8</v>
       </c>
       <c r="E36" s="27">
-        <f>C36+D36</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="F36" s="24">
-        <f>(E36/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>53.333333333333336</v>
       </c>
       <c r="G36" s="18" t="str">
-        <f>IF(F36&gt;94,"A+",IF(F36&gt;84,"A",IF(F36&gt;79,"A-",IF(F36&gt;74,"B+",IF(F36&gt;69,"B",IF(F36&gt;64,"B-",IF(F36&gt;59,"C+",IF(F36&gt;54,"C",IF(F36&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
     </row>
@@ -13320,15 +14893,15 @@
         <v>9</v>
       </c>
       <c r="E37" s="27">
-        <f>C37+D37</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="F37" s="24">
-        <f>(E37/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>93.333333333333329</v>
       </c>
       <c r="G37" s="18" t="str">
-        <f>IF(F37&gt;94,"A+",IF(F37&gt;84,"A",IF(F37&gt;79,"A-",IF(F37&gt;74,"B+",IF(F37&gt;69,"B",IF(F37&gt;64,"B-",IF(F37&gt;59,"C+",IF(F37&gt;54,"C",IF(F37&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -13348,15 +14921,15 @@
         <v>8</v>
       </c>
       <c r="E38" s="27">
-        <f>C38+D38</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F38" s="24">
-        <f>(E38/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G38" s="18" t="str">
-        <f>IF(F38&gt;94,"A+",IF(F38&gt;84,"A",IF(F38&gt;79,"A-",IF(F38&gt;74,"B+",IF(F38&gt;69,"B",IF(F38&gt;64,"B-",IF(F38&gt;59,"C+",IF(F38&gt;54,"C",IF(F38&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13376,15 +14949,15 @@
         <v>9</v>
       </c>
       <c r="E39" s="27">
-        <f>C39+D39</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F39" s="24">
-        <f>(E39/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G39" s="18" t="str">
-        <f>IF(F39&gt;94,"A+",IF(F39&gt;84,"A",IF(F39&gt;79,"A-",IF(F39&gt;74,"B+",IF(F39&gt;69,"B",IF(F39&gt;64,"B-",IF(F39&gt;59,"C+",IF(F39&gt;54,"C",IF(F39&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13404,15 +14977,15 @@
         <v>9</v>
       </c>
       <c r="E40" s="27">
-        <f>C40+D40</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="F40" s="24">
-        <f>(E40/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G40" s="18" t="str">
-        <f>IF(F40&gt;94,"A+",IF(F40&gt;84,"A",IF(F40&gt;79,"A-",IF(F40&gt;74,"B+",IF(F40&gt;69,"B",IF(F40&gt;64,"B-",IF(F40&gt;59,"C+",IF(F40&gt;54,"C",IF(F40&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
@@ -13432,15 +15005,15 @@
         <v>8</v>
       </c>
       <c r="E41" s="27">
-        <f>C41+D41</f>
+        <f t="shared" si="3"/>
         <v>11.5</v>
       </c>
       <c r="F41" s="24">
-        <f>(E41/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>76.666666666666671</v>
       </c>
       <c r="G41" s="18" t="str">
-        <f>IF(F41&gt;94,"A+",IF(F41&gt;84,"A",IF(F41&gt;79,"A-",IF(F41&gt;74,"B+",IF(F41&gt;69,"B",IF(F41&gt;64,"B-",IF(F41&gt;59,"C+",IF(F41&gt;54,"C",IF(F41&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B+</v>
       </c>
     </row>
@@ -13460,15 +15033,15 @@
         <v>0</v>
       </c>
       <c r="E42" s="27">
-        <f>C42+D42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F42" s="24">
-        <f>(E42/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G42" s="18" t="str">
-        <f>IF(F42&gt;94,"A+",IF(F42&gt;84,"A",IF(F42&gt;79,"A-",IF(F42&gt;74,"B+",IF(F42&gt;69,"B",IF(F42&gt;64,"B-",IF(F42&gt;59,"C+",IF(F42&gt;54,"C",IF(F42&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
     </row>
@@ -13488,15 +15061,15 @@
         <v>9</v>
       </c>
       <c r="E43" s="27">
-        <f>C43+D43</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="F43" s="24">
-        <f>(E43/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G43" s="18" t="str">
-        <f>IF(F43&gt;94,"A+",IF(F43&gt;84,"A",IF(F43&gt;79,"A-",IF(F43&gt;74,"B+",IF(F43&gt;69,"B",IF(F43&gt;64,"B-",IF(F43&gt;59,"C+",IF(F43&gt;54,"C",IF(F43&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
@@ -13516,15 +15089,15 @@
         <v>8</v>
       </c>
       <c r="E44" s="27">
-        <f>C44+D44</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F44" s="24">
-        <f>(E44/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G44" s="18" t="str">
-        <f>IF(F44&gt;94,"A+",IF(F44&gt;84,"A",IF(F44&gt;79,"A-",IF(F44&gt;74,"B+",IF(F44&gt;69,"B",IF(F44&gt;64,"B-",IF(F44&gt;59,"C+",IF(F44&gt;54,"C",IF(F44&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13544,15 +15117,15 @@
         <v>8</v>
       </c>
       <c r="E45" s="27">
-        <f>C45+D45</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="F45" s="24">
-        <f>(E45/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>83.333333333333343</v>
       </c>
       <c r="G45" s="18" t="str">
-        <f>IF(F45&gt;94,"A+",IF(F45&gt;84,"A",IF(F45&gt;79,"A-",IF(F45&gt;74,"B+",IF(F45&gt;69,"B",IF(F45&gt;64,"B-",IF(F45&gt;59,"C+",IF(F45&gt;54,"C",IF(F45&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13572,15 +15145,15 @@
         <v>6</v>
       </c>
       <c r="E46" s="27">
-        <f>C46+D46</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="F46" s="24">
-        <f>(E46/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G46" s="18" t="str">
-        <f>IF(F46&gt;94,"A+",IF(F46&gt;84,"A",IF(F46&gt;79,"A-",IF(F46&gt;74,"B+",IF(F46&gt;69,"B",IF(F46&gt;64,"B-",IF(F46&gt;59,"C+",IF(F46&gt;54,"C",IF(F46&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>C+</v>
       </c>
     </row>
@@ -13600,15 +15173,15 @@
         <v>9</v>
       </c>
       <c r="E47" s="27">
-        <f>C47+D47</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="F47" s="24">
-        <f>(E47/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>93.333333333333329</v>
       </c>
       <c r="G47" s="18" t="str">
-        <f>IF(F47&gt;94,"A+",IF(F47&gt;84,"A",IF(F47&gt;79,"A-",IF(F47&gt;74,"B+",IF(F47&gt;69,"B",IF(F47&gt;64,"B-",IF(F47&gt;59,"C+",IF(F47&gt;54,"C",IF(F47&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A</v>
       </c>
     </row>
@@ -13628,15 +15201,15 @@
         <v>8</v>
       </c>
       <c r="E48" s="27">
-        <f>C48+D48</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="F48" s="24">
-        <f>(E48/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>73.333333333333329</v>
       </c>
       <c r="G48" s="18" t="str">
-        <f>IF(F48&gt;94,"A+",IF(F48&gt;84,"A",IF(F48&gt;79,"A-",IF(F48&gt;74,"B+",IF(F48&gt;69,"B",IF(F48&gt;64,"B-",IF(F48&gt;59,"C+",IF(F48&gt;54,"C",IF(F48&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
@@ -13656,15 +15229,15 @@
         <v>9</v>
       </c>
       <c r="E49" s="14">
-        <f>C49+D49</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F49" s="13">
-        <f>(E49/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G49" s="12" t="str">
-        <f>IF(F49&gt;94,"A+",IF(F49&gt;84,"A",IF(F49&gt;79,"A-",IF(F49&gt;74,"B+",IF(F49&gt;69,"B",IF(F49&gt;64,"B-",IF(F49&gt;59,"C+",IF(F49&gt;54,"C",IF(F49&gt;49,"D","F")))))))))</f>
+        <f t="shared" si="2"/>
         <v>A-</v>
       </c>
     </row>
@@ -13676,11 +15249,11 @@
         <v>10</v>
       </c>
       <c r="E50" s="11">
-        <f>C50+D50</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="F50" s="24">
-        <f>(E50/E$50)*100</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>

</xml_diff>